<commit_message>
- Test suite became fully independent of any third-party libraries. Just checkout and build it. - DataObjects.Net is updated to the latest version (v4.1 RC).
</commit_message>
<xml_diff>
--- a/_Documents/ORMBattle.NET Test Results.xlsx
+++ b/_Documents/ORMBattle.NET Test Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="101">
   <si>
     <t>SqlClient</t>
   </si>
@@ -1089,7 +1089,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1209,9 +1209,6 @@
     <xf numFmtId="49" fontId="13" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="17" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="13" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="17" fillId="45" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="17" fillId="45" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1230,7 +1227,6 @@
     <xf numFmtId="49" fontId="13" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="45" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="24" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2425,25 +2421,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115910912"/>
-        <c:axId val="115920896"/>
+        <c:axId val="115882240"/>
+        <c:axId val="115912704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115910912"/>
+        <c:axId val="115882240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115920896"/>
+        <c:crossAx val="115912704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115920896"/>
+        <c:axId val="115912704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2453,7 +2449,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115910912"/>
+        <c:crossAx val="115882240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2465,7 +2461,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2644,25 +2640,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115491584"/>
-        <c:axId val="115493120"/>
+        <c:axId val="116077312"/>
+        <c:axId val="116078848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115491584"/>
+        <c:axId val="116077312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115493120"/>
+        <c:crossAx val="116078848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115493120"/>
+        <c:axId val="116078848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2671,7 +2667,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115491584"/>
+        <c:crossAx val="116077312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2683,7 +2679,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2903,25 +2899,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115522944"/>
-        <c:axId val="116069504"/>
+        <c:axId val="116100480"/>
+        <c:axId val="116126848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115522944"/>
+        <c:axId val="116100480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116069504"/>
+        <c:crossAx val="116126848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116069504"/>
+        <c:axId val="116126848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2930,7 +2926,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115522944"/>
+        <c:crossAx val="116100480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2942,7 +2938,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3053,25 +3049,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="116078080"/>
-        <c:axId val="116091136"/>
+        <c:axId val="115480064"/>
+        <c:axId val="115493120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116078080"/>
+        <c:axId val="115480064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116091136"/>
+        <c:crossAx val="115493120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116091136"/>
+        <c:axId val="115493120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3080,7 +3076,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116078080"/>
+        <c:crossAx val="115480064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3092,7 +3088,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000555" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000555" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3203,25 +3199,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="116115328"/>
-        <c:axId val="116116864"/>
+        <c:axId val="115513216"/>
+        <c:axId val="115514752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116115328"/>
+        <c:axId val="115513216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116116864"/>
+        <c:crossAx val="115514752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116116864"/>
+        <c:axId val="115514752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3232,7 +3228,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116115328"/>
+        <c:crossAx val="115513216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3245,7 +3241,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3560,25 +3556,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="116234880"/>
-        <c:axId val="116240768"/>
+        <c:axId val="116226688"/>
+        <c:axId val="116232576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116234880"/>
+        <c:axId val="116226688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116240768"/>
+        <c:crossAx val="116232576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116240768"/>
+        <c:axId val="116232576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3587,7 +3583,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116234880"/>
+        <c:crossAx val="116226688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3609,7 +3605,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000577" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000577" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3924,25 +3920,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="116340224"/>
-        <c:axId val="116341760"/>
+        <c:axId val="116262400"/>
+        <c:axId val="116263936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="116340224"/>
+        <c:axId val="116262400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116341760"/>
+        <c:crossAx val="116263936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116341760"/>
+        <c:axId val="116263936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3952,7 +3948,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116340224"/>
+        <c:crossAx val="116262400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3964,7 +3960,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4497,10 +4493,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K137"/>
+  <dimension ref="A1:M137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K64" sqref="K64"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4601,13 +4597,13 @@
       <c r="C6" s="53">
         <v>5</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="65">
         <v>0</v>
       </c>
-      <c r="F6" s="67" t="s">
+      <c r="F6" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="53">
@@ -4619,7 +4615,7 @@
       <c r="I6" s="53">
         <v>1</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K6" s="47" t="s">
@@ -4636,13 +4632,13 @@
       <c r="C7" s="53">
         <v>6</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="69">
+      <c r="E7" s="66">
         <v>3</v>
       </c>
-      <c r="F7" s="67" t="s">
+      <c r="F7" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="53">
@@ -4654,7 +4650,7 @@
       <c r="I7" s="53">
         <v>4</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K7" s="47" t="s">
@@ -4671,13 +4667,13 @@
       <c r="C8" s="53">
         <v>6</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="69">
+      <c r="E8" s="66">
         <v>1</v>
       </c>
-      <c r="F8" s="67" t="s">
+      <c r="F8" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="53">
@@ -4689,7 +4685,7 @@
       <c r="I8" s="53">
         <v>6</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K8" s="47" t="s">
@@ -4706,13 +4702,13 @@
       <c r="C9" s="53">
         <v>9</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="66">
         <v>4</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="53">
@@ -4724,7 +4720,7 @@
       <c r="I9" s="53">
         <v>5</v>
       </c>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="47" t="s">
@@ -4741,13 +4737,13 @@
       <c r="C10" s="53">
         <v>12</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="69">
+      <c r="E10" s="66">
         <v>4.2</v>
       </c>
-      <c r="F10" s="67" t="s">
+      <c r="F10" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="53">
@@ -4759,7 +4755,7 @@
       <c r="I10" s="53">
         <v>2</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="47" t="s">
@@ -4776,13 +4772,13 @@
       <c r="C11" s="53">
         <v>10.199999999999999</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="69">
+      <c r="E11" s="66">
         <v>1</v>
       </c>
-      <c r="F11" s="67" t="s">
+      <c r="F11" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="53">
@@ -4794,7 +4790,7 @@
       <c r="I11" s="53">
         <v>5</v>
       </c>
-      <c r="J11" s="67" t="s">
+      <c r="J11" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K11" s="47" t="s">
@@ -4811,13 +4807,13 @@
       <c r="C12" s="53">
         <v>4</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="69">
+      <c r="E12" s="66">
         <v>1</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="53">
@@ -4829,7 +4825,7 @@
       <c r="I12" s="53">
         <v>4</v>
       </c>
-      <c r="J12" s="67" t="s">
+      <c r="J12" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K12" s="47" t="s">
@@ -4846,13 +4842,13 @@
       <c r="C13" s="53">
         <v>8</v>
       </c>
-      <c r="D13" s="83" t="s">
+      <c r="D13" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="69">
+      <c r="E13" s="66">
         <v>3.2</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="53">
@@ -4864,7 +4860,7 @@
       <c r="I13" s="53">
         <v>6</v>
       </c>
-      <c r="J13" s="67" t="s">
+      <c r="J13" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K13" s="47" t="s">
@@ -4881,13 +4877,13 @@
       <c r="C14" s="53">
         <v>13</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D14" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="69">
+      <c r="E14" s="66">
         <v>2</v>
       </c>
-      <c r="F14" s="67" t="s">
+      <c r="F14" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="53">
@@ -4899,7 +4895,7 @@
       <c r="I14" s="53">
         <v>8.1</v>
       </c>
-      <c r="J14" s="67" t="s">
+      <c r="J14" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K14" s="47" t="s">
@@ -4916,13 +4912,13 @@
       <c r="C15" s="53">
         <v>4</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="69">
+      <c r="E15" s="66">
         <v>0</v>
       </c>
-      <c r="F15" s="67" t="s">
+      <c r="F15" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="53">
@@ -4934,7 +4930,7 @@
       <c r="I15" s="53">
         <v>2</v>
       </c>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K15" s="47" t="s">
@@ -4951,13 +4947,13 @@
       <c r="C16" s="53">
         <v>9</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="D16" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="69">
+      <c r="E16" s="66">
         <v>0</v>
       </c>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="53">
@@ -4969,7 +4965,7 @@
       <c r="I16" s="53">
         <v>9</v>
       </c>
-      <c r="J16" s="67" t="s">
+      <c r="J16" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K16" s="47" t="s">
@@ -4986,13 +4982,13 @@
       <c r="C17" s="53">
         <v>21</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="69">
+      <c r="E17" s="66">
         <v>9</v>
       </c>
-      <c r="F17" s="67" t="s">
+      <c r="F17" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="53">
@@ -5004,7 +5000,7 @@
       <c r="I17" s="53">
         <v>11</v>
       </c>
-      <c r="J17" s="67" t="s">
+      <c r="J17" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K17" s="47" t="s">
@@ -5021,13 +5017,13 @@
       <c r="C18" s="53">
         <v>5</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="69">
+      <c r="E18" s="66">
         <v>1</v>
       </c>
-      <c r="F18" s="67" t="s">
+      <c r="F18" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="53">
@@ -5039,7 +5035,7 @@
       <c r="I18" s="53">
         <v>2</v>
       </c>
-      <c r="J18" s="67" t="s">
+      <c r="J18" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K18" s="47" t="s">
@@ -5056,13 +5052,13 @@
       <c r="C19" s="53">
         <v>5</v>
       </c>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="69">
+      <c r="E19" s="66">
         <v>1</v>
       </c>
-      <c r="F19" s="67" t="s">
+      <c r="F19" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="53">
@@ -5074,7 +5070,7 @@
       <c r="I19" s="53">
         <v>2</v>
       </c>
-      <c r="J19" s="67" t="s">
+      <c r="J19" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K19" s="47" t="s">
@@ -5086,7 +5082,7 @@
       <c r="B20" s="58"/>
       <c r="C20" s="58"/>
       <c r="D20" s="58"/>
-      <c r="E20" s="70"/>
+      <c r="E20" s="67"/>
       <c r="F20" s="58"/>
       <c r="G20" s="58"/>
       <c r="H20" s="58"/>
@@ -5101,7 +5097,7 @@
       <c r="B21" s="52"/>
       <c r="C21" s="52"/>
       <c r="D21" s="52"/>
-      <c r="E21" s="71"/>
+      <c r="E21" s="68"/>
       <c r="F21" s="52"/>
       <c r="G21" s="52"/>
       <c r="H21" s="52"/>
@@ -5113,27 +5109,33 @@
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="59">
+      <c r="B22" s="63">
         <v>0</v>
       </c>
-      <c r="C22" s="60">
+      <c r="C22" s="63">
         <v>117</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="72">
+      <c r="D22" s="80" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="69">
         <v>117</v>
       </c>
-      <c r="F22" s="61"/>
-      <c r="G22" s="59">
+      <c r="F22" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="63">
         <v>117</v>
       </c>
-      <c r="H22" s="59">
+      <c r="H22" s="63">
         <v>117</v>
       </c>
-      <c r="I22" s="59">
+      <c r="I22" s="63">
         <v>117</v>
       </c>
-      <c r="J22" s="60"/>
+      <c r="J22" s="62" t="s">
+        <v>13</v>
+      </c>
       <c r="K22" s="47" t="s">
         <v>38</v>
       </c>
@@ -5142,31 +5144,31 @@
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="66">
+      <c r="B23" s="63">
         <v>0</v>
       </c>
-      <c r="C23" s="66">
+      <c r="C23" s="63">
         <v>117</v>
       </c>
-      <c r="D23" s="84" t="s">
+      <c r="D23" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="73">
+      <c r="E23" s="69">
         <v>87</v>
       </c>
-      <c r="F23" s="65" t="s">
+      <c r="F23" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="66">
+      <c r="G23" s="63">
         <v>41</v>
       </c>
-      <c r="H23" s="66">
+      <c r="H23" s="63">
         <v>35</v>
       </c>
-      <c r="I23" s="66">
+      <c r="I23" s="63">
         <v>50</v>
       </c>
-      <c r="J23" s="65" t="s">
+      <c r="J23" s="62" t="s">
         <v>13</v>
       </c>
       <c r="K23" s="47" t="s">
@@ -5183,13 +5185,13 @@
       <c r="C24" s="53">
         <v>117</v>
       </c>
-      <c r="D24" s="83" t="s">
+      <c r="D24" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="69">
+      <c r="E24" s="66">
         <v>30</v>
       </c>
-      <c r="F24" s="67" t="s">
+      <c r="F24" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="53">
@@ -5201,7 +5203,7 @@
       <c r="I24" s="53">
         <v>67</v>
       </c>
-      <c r="J24" s="67" t="s">
+      <c r="J24" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K24" s="47" t="s">
@@ -5218,13 +5220,13 @@
       <c r="C25" s="53">
         <v>117</v>
       </c>
-      <c r="D25" s="83" t="s">
+      <c r="D25" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="69">
+      <c r="E25" s="66">
         <v>26</v>
       </c>
-      <c r="F25" s="67" t="s">
+      <c r="F25" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="53">
@@ -5236,7 +5238,7 @@
       <c r="I25" s="53">
         <v>66</v>
       </c>
-      <c r="J25" s="67" t="s">
+      <c r="J25" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K25" s="47" t="s">
@@ -5253,13 +5255,13 @@
       <c r="C26" s="53">
         <v>15</v>
       </c>
-      <c r="D26" s="83" t="s">
+      <c r="D26" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="69">
+      <c r="E26" s="66">
         <v>4</v>
       </c>
-      <c r="F26" s="67" t="s">
+      <c r="F26" s="64" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="53">
@@ -5271,7 +5273,7 @@
       <c r="I26" s="53">
         <v>1</v>
       </c>
-      <c r="J26" s="67" t="s">
+      <c r="J26" s="64" t="s">
         <v>13</v>
       </c>
       <c r="K26" s="47" t="s">
@@ -5288,13 +5290,13 @@
       <c r="C27" s="44">
         <v>100</v>
       </c>
-      <c r="D27" s="84" t="s">
+      <c r="D27" s="80" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="22">
         <v>74.400000000000006</v>
       </c>
-      <c r="F27" s="65" t="s">
+      <c r="F27" s="62" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="43">
@@ -5306,7 +5308,7 @@
       <c r="I27" s="43">
         <v>42.7</v>
       </c>
-      <c r="J27" s="65" t="s">
+      <c r="J27" s="62" t="s">
         <v>13</v>
       </c>
       <c r="K27" s="47" t="s">
@@ -5377,12 +5379,12 @@
       <c r="A32" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="74" t="s">
+      <c r="B32" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
       <c r="F32" s="45"/>
       <c r="G32" s="45"/>
       <c r="H32" s="45"/>
@@ -5393,12 +5395,12 @@
       <c r="A33" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="74" t="s">
+      <c r="B33" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
       <c r="F33" s="45"/>
       <c r="G33" s="45"/>
       <c r="H33" s="45"/>
@@ -5409,12 +5411,12 @@
       <c r="A34" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="74" t="s">
+      <c r="B34" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
       <c r="F34" s="45"/>
       <c r="G34" s="45"/>
       <c r="H34" s="45"/>
@@ -5423,15 +5425,15 @@
     </row>
     <row r="35" spans="1:11" s="34" customFormat="1">
       <c r="A35" s="5"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="63"/>
-      <c r="J35" s="63"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
       <c r="K35" s="19"/>
     </row>
     <row r="36" spans="1:11" s="38" customFormat="1">
@@ -5448,37 +5450,37 @@
       </c>
     </row>
     <row r="37" spans="1:11" s="34" customFormat="1" ht="87.75">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="77" t="s">
+      <c r="B37" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="77" t="s">
+      <c r="C37" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="77" t="s">
+      <c r="D37" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="E37" s="77" t="s">
+      <c r="E37" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="77" t="s">
+      <c r="F37" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="77" t="s">
+      <c r="G37" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="H37" s="77" t="s">
+      <c r="H37" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I37" s="77" t="s">
+      <c r="I37" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="J37" s="77" t="s">
+      <c r="J37" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="K37" s="77" t="s">
+      <c r="K37" s="73" t="s">
         <v>21</v>
       </c>
     </row>
@@ -5536,7 +5538,7 @@
       </c>
       <c r="B40" s="54"/>
       <c r="C40" s="54"/>
-      <c r="D40" s="79"/>
+      <c r="D40" s="75"/>
       <c r="E40" s="57"/>
       <c r="F40" s="57"/>
       <c r="G40" s="57"/>
@@ -5683,7 +5685,7 @@
       </c>
       <c r="B45" s="54"/>
       <c r="C45" s="54"/>
-      <c r="D45" s="79"/>
+      <c r="D45" s="75"/>
       <c r="E45" s="57"/>
       <c r="F45" s="57"/>
       <c r="G45" s="57"/>
@@ -5858,7 +5860,7 @@
       </c>
       <c r="B52" s="48"/>
       <c r="C52" s="48"/>
-      <c r="D52" s="80"/>
+      <c r="D52" s="76"/>
       <c r="E52" s="55"/>
       <c r="F52" s="55"/>
       <c r="G52" s="55"/>
@@ -5972,7 +5974,7 @@
       </c>
       <c r="B56" s="48"/>
       <c r="C56" s="48"/>
-      <c r="D56" s="80"/>
+      <c r="D56" s="76"/>
       <c r="E56" s="55"/>
       <c r="F56" s="55"/>
       <c r="G56" s="55"/>
@@ -6119,7 +6121,7 @@
       </c>
       <c r="B61" s="48"/>
       <c r="C61" s="48"/>
-      <c r="D61" s="80"/>
+      <c r="D61" s="76"/>
       <c r="E61" s="55"/>
       <c r="F61" s="55"/>
       <c r="G61" s="55"/>
@@ -6165,29 +6167,29 @@
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B63" s="66">
+      <c r="B63" s="63">
         <v>0</v>
       </c>
-      <c r="C63" s="66"/>
-      <c r="D63" s="81" t="s">
+      <c r="C63" s="63"/>
+      <c r="D63" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="E63" s="65">
+      <c r="E63" s="62">
         <v>465073</v>
       </c>
-      <c r="F63" s="65">
+      <c r="F63" s="62">
         <v>751879</v>
       </c>
-      <c r="G63" s="65">
+      <c r="G63" s="62">
         <v>422332</v>
       </c>
-      <c r="H63" s="65">
+      <c r="H63" s="62">
         <v>53329</v>
       </c>
-      <c r="I63" s="65">
+      <c r="I63" s="62">
         <v>234329</v>
       </c>
-      <c r="J63" s="65">
+      <c r="J63" s="62">
         <v>57411</v>
       </c>
       <c r="K63" s="47" t="s">
@@ -6196,18 +6198,18 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="5"/>
-      <c r="B64" s="62"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="62"/>
-      <c r="E64" s="62"/>
-      <c r="F64" s="64"/>
-      <c r="G64" s="64"/>
-      <c r="H64" s="64"/>
-      <c r="I64" s="64"/>
-      <c r="J64" s="62"/>
-      <c r="K64" s="62"/>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="B64" s="59"/>
+      <c r="C64" s="59"/>
+      <c r="D64" s="59"/>
+      <c r="E64" s="59"/>
+      <c r="F64" s="61"/>
+      <c r="G64" s="61"/>
+      <c r="H64" s="61"/>
+      <c r="I64" s="61"/>
+      <c r="J64" s="59"/>
+      <c r="K64" s="59"/>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" s="8" t="s">
         <v>12</v>
       </c>
@@ -6222,20 +6224,20 @@
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:13">
       <c r="A66" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B66" s="26"/>
       <c r="C66" s="56"/>
-      <c r="D66" s="82" t="s">
+      <c r="D66" s="78" t="s">
         <v>13</v>
       </c>
       <c r="E66" s="13">
+        <v>58171</v>
+      </c>
+      <c r="F66" s="13">
         <v>10350</v>
-      </c>
-      <c r="F66" s="13">
-        <v>58171</v>
       </c>
       <c r="G66" s="13">
         <v>14762</v>
@@ -6253,21 +6255,22 @@
       <c r="K66" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="M66" s="34"/>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B67" s="26"/>
       <c r="C67" s="56"/>
-      <c r="D67" s="82" t="s">
+      <c r="D67" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E67" s="23">
+      <c r="E67" s="20">
+        <v>126449</v>
+      </c>
+      <c r="F67" s="23">
         <v>0</v>
-      </c>
-      <c r="F67" s="23">
-        <v>126449</v>
       </c>
       <c r="G67" s="23">
         <v>32121</v>
@@ -6284,21 +6287,22 @@
       <c r="K67" s="24">
         <v>124093</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="M67" s="34"/>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="26"/>
       <c r="C68" s="56"/>
-      <c r="D68" s="82" t="s">
+      <c r="D68" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E68" s="13">
+      <c r="E68" s="20">
+        <v>2879448</v>
+      </c>
+      <c r="F68" s="13">
         <v>1102848</v>
-      </c>
-      <c r="F68" s="20">
-        <v>2879448</v>
       </c>
       <c r="G68" s="20">
         <v>347136</v>
@@ -6315,8 +6319,9 @@
       <c r="K68" s="21">
         <v>280064</v>
       </c>
-    </row>
-    <row r="69" spans="1:11">
+      <c r="M68" s="34"/>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -6329,7 +6334,7 @@
       <c r="J69" s="14"/>
       <c r="K69" s="14"/>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:13">
       <c r="A70" s="15" t="s">
         <v>2</v>
       </c>
@@ -6348,7 +6353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="34" customFormat="1">
+    <row r="71" spans="1:13" s="34" customFormat="1">
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -6361,7 +6366,7 @@
       <c r="J71" s="14"/>
       <c r="K71" s="14"/>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:13">
       <c r="A72" s="8" t="s">
         <v>74</v>
       </c>
@@ -6376,86 +6381,86 @@
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
     </row>
-    <row r="73" spans="1:11" s="34" customFormat="1">
+    <row r="73" spans="1:13" s="34" customFormat="1">
       <c r="A73" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B73" s="74" t="s">
+      <c r="B73" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="C73" s="74"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="70"/>
+      <c r="E73" s="70"/>
       <c r="F73" s="45"/>
       <c r="G73" s="45"/>
       <c r="H73" s="45"/>
       <c r="I73" s="45"/>
       <c r="K73" s="45"/>
     </row>
-    <row r="74" spans="1:11" s="34" customFormat="1">
+    <row r="74" spans="1:13" s="34" customFormat="1">
       <c r="A74" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B74" s="74" t="s">
+      <c r="B74" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="C74" s="74"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="70"/>
+      <c r="E74" s="70"/>
       <c r="F74" s="45"/>
       <c r="G74" s="45"/>
       <c r="H74" s="45"/>
       <c r="I74" s="45"/>
       <c r="K74" s="45"/>
     </row>
-    <row r="75" spans="1:11" s="34" customFormat="1">
+    <row r="75" spans="1:13" s="34" customFormat="1">
       <c r="A75" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B75" s="74" t="s">
+      <c r="B75" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="C75" s="74"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="70"/>
+      <c r="E75" s="70"/>
       <c r="F75" s="45"/>
       <c r="G75" s="45"/>
       <c r="H75" s="45"/>
       <c r="I75" s="45"/>
       <c r="K75" s="45"/>
     </row>
-    <row r="76" spans="1:11" s="34" customFormat="1">
+    <row r="76" spans="1:13" s="34" customFormat="1">
       <c r="A76" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B76" s="74" t="s">
+      <c r="B76" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="74"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="74"/>
-      <c r="H76" s="74"/>
-      <c r="I76" s="74"/>
-      <c r="J76" s="75"/>
-      <c r="K76" s="74"/>
-    </row>
-    <row r="77" spans="1:11" s="31" customFormat="1">
+      <c r="C76" s="70"/>
+      <c r="D76" s="70"/>
+      <c r="E76" s="70"/>
+      <c r="F76" s="70"/>
+      <c r="G76" s="70"/>
+      <c r="H76" s="70"/>
+      <c r="I76" s="70"/>
+      <c r="J76" s="71"/>
+      <c r="K76" s="70"/>
+    </row>
+    <row r="77" spans="1:13" s="31" customFormat="1">
       <c r="A77" s="30"/>
       <c r="B77" s="37"/>
       <c r="C77" s="37"/>
       <c r="E77" s="38"/>
       <c r="J77" s="38"/>
     </row>
-    <row r="78" spans="1:11" s="38" customFormat="1">
+    <row r="78" spans="1:13" s="38" customFormat="1">
       <c r="A78" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B78" s="37"/>
       <c r="C78" s="37"/>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:13">
       <c r="A79" s="2" t="s">
         <v>8</v>
       </c>
@@ -6498,7 +6503,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K59">
-    <cfRule type="colorScale" priority="1960">
+    <cfRule type="colorScale" priority="1964">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6510,7 +6515,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59">
-    <cfRule type="colorScale" priority="1956">
+    <cfRule type="colorScale" priority="1960">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -6518,12 +6523,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="59" priority="1957" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="58" priority="1958" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="57" priority="1959" rank="1"/>
+    <cfRule type="top10" dxfId="59" priority="1961" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="58" priority="1962" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="57" priority="1963" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K60">
-    <cfRule type="colorScale" priority="1433">
+    <cfRule type="colorScale" priority="1437">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -6531,15 +6536,15 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="56" priority="1434" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="55" priority="1435" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="54" priority="1436" rank="1"/>
+    <cfRule type="top10" dxfId="56" priority="1438" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="55" priority="1439" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="54" priority="1440" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61">
-    <cfRule type="top10" dxfId="53" priority="1432" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="53" priority="1436" percent="1" rank="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61">
-    <cfRule type="colorScale" priority="1425">
+    <cfRule type="colorScale" priority="1429">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -6547,12 +6552,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="52" priority="1426" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="51" priority="1427" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="50" priority="1428" rank="1"/>
+    <cfRule type="top10" dxfId="52" priority="1430" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="51" priority="1431" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="50" priority="1432" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K60">
-    <cfRule type="colorScale" priority="1412">
+    <cfRule type="colorScale" priority="1416">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6564,7 +6569,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61">
-    <cfRule type="colorScale" priority="1411">
+    <cfRule type="colorScale" priority="1415">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6576,7 +6581,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="colorScale" priority="1401">
+    <cfRule type="colorScale" priority="1405">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6588,7 +6593,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70:K70">
-    <cfRule type="colorScale" priority="3246">
+    <cfRule type="colorScale" priority="3250">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6600,7 +6605,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69:K69">
-    <cfRule type="colorScale" priority="3598">
+    <cfRule type="colorScale" priority="3602">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6612,7 +6617,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="colorScale" priority="3822">
+    <cfRule type="colorScale" priority="3826">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6624,7 +6629,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70">
-    <cfRule type="colorScale" priority="842">
+    <cfRule type="colorScale" priority="846">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -6632,12 +6637,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="49" priority="843" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="48" priority="844" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="47" priority="845" rank="1"/>
+    <cfRule type="top10" dxfId="49" priority="847" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="48" priority="848" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="47" priority="849" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70">
-    <cfRule type="colorScale" priority="841">
+    <cfRule type="colorScale" priority="845">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6649,7 +6654,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70">
-    <cfRule type="colorScale" priority="837">
+    <cfRule type="colorScale" priority="841">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -6657,12 +6662,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="46" priority="838" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="45" priority="839" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="44" priority="840" rank="1"/>
+    <cfRule type="top10" dxfId="46" priority="842" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="45" priority="843" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="44" priority="844" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70">
-    <cfRule type="colorScale" priority="836">
+    <cfRule type="colorScale" priority="840">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6674,7 +6679,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="colorScale" priority="812">
+    <cfRule type="colorScale" priority="816">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -6682,12 +6687,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="43" priority="813" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="42" priority="814" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="41" priority="815" rank="1"/>
+    <cfRule type="top10" dxfId="43" priority="817" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="42" priority="818" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="41" priority="819" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="colorScale" priority="811">
+    <cfRule type="colorScale" priority="815">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6699,7 +6704,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="colorScale" priority="806">
+    <cfRule type="colorScale" priority="810">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -6707,12 +6712,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="40" priority="807" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="39" priority="808" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="38" priority="809" rank="1"/>
+    <cfRule type="top10" dxfId="40" priority="811" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="39" priority="812" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="38" priority="813" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="colorScale" priority="805">
+    <cfRule type="colorScale" priority="809">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6724,7 +6729,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="colorScale" priority="4737">
+    <cfRule type="colorScale" priority="4741">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6736,7 +6741,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70:G70">
-    <cfRule type="colorScale" priority="4745">
+    <cfRule type="colorScale" priority="4749">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6748,7 +6753,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70">
-    <cfRule type="colorScale" priority="4750">
+    <cfRule type="colorScale" priority="4754">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6760,7 +6765,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:K59 K6:K19 K39:K49 K22:K30 K35">
-    <cfRule type="colorScale" priority="5088">
+    <cfRule type="colorScale" priority="5092">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6772,7 +6777,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:K59">
-    <cfRule type="colorScale" priority="5093">
+    <cfRule type="colorScale" priority="5097">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6784,7 +6789,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:J18">
-    <cfRule type="colorScale" priority="97">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6796,7 +6801,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:J19">
-    <cfRule type="colorScale" priority="98">
+    <cfRule type="colorScale" priority="102">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6808,7 +6813,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:J25">
-    <cfRule type="colorScale" priority="102">
+    <cfRule type="colorScale" priority="106">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6820,7 +6825,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:J26">
-    <cfRule type="colorScale" priority="103">
+    <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6832,7 +6837,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6">
-    <cfRule type="colorScale" priority="85">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6844,7 +6849,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:J7">
-    <cfRule type="colorScale" priority="86">
+    <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6856,7 +6861,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:J8">
-    <cfRule type="colorScale" priority="87">
+    <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6868,7 +6873,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:J9">
-    <cfRule type="colorScale" priority="88">
+    <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6880,7 +6885,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:J10">
-    <cfRule type="colorScale" priority="89">
+    <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6892,7 +6897,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:J11">
-    <cfRule type="colorScale" priority="90">
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6904,7 +6909,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:J12">
-    <cfRule type="colorScale" priority="91">
+    <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6916,7 +6921,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:J13">
-    <cfRule type="colorScale" priority="92">
+    <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6928,7 +6933,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J14">
-    <cfRule type="colorScale" priority="93">
+    <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6940,7 +6945,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:J15">
-    <cfRule type="colorScale" priority="94">
+    <cfRule type="colorScale" priority="98">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6952,7 +6957,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:J16">
-    <cfRule type="colorScale" priority="95">
+    <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6964,7 +6969,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:J17">
-    <cfRule type="colorScale" priority="96">
+    <cfRule type="colorScale" priority="100">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6976,7 +6981,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:J23">
-    <cfRule type="colorScale" priority="99">
+    <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -6988,7 +6993,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:J24">
-    <cfRule type="colorScale" priority="100">
+    <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7000,7 +7005,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:J27">
-    <cfRule type="colorScale" priority="103">
+    <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7012,7 +7017,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:J39">
-    <cfRule type="colorScale" priority="115">
+    <cfRule type="colorScale" priority="119">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7024,7 +7029,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:J41">
-    <cfRule type="colorScale" priority="117">
+    <cfRule type="colorScale" priority="121">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7036,7 +7041,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:J42">
-    <cfRule type="colorScale" priority="118">
+    <cfRule type="colorScale" priority="122">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7048,7 +7053,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:J43">
-    <cfRule type="colorScale" priority="119">
+    <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7060,7 +7065,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:J44">
-    <cfRule type="colorScale" priority="120">
+    <cfRule type="colorScale" priority="124">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7072,7 +7077,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:J46">
-    <cfRule type="colorScale" priority="122">
+    <cfRule type="colorScale" priority="126">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7084,7 +7089,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:J47">
-    <cfRule type="colorScale" priority="123">
+    <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7096,7 +7101,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:J48">
-    <cfRule type="colorScale" priority="124">
+    <cfRule type="colorScale" priority="128">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7108,7 +7113,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:J49">
-    <cfRule type="colorScale" priority="125">
+    <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7120,7 +7125,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53:J53">
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7132,7 +7137,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:J54">
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7144,7 +7149,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55:J55">
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7156,7 +7161,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57:J57">
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7168,7 +7173,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58:J58">
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7180,7 +7185,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59:J59">
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7192,7 +7197,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60:J60">
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7204,7 +7209,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:J62">
-    <cfRule type="colorScale" priority="107">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7216,7 +7221,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62:K63">
-    <cfRule type="colorScale" priority="5115">
+    <cfRule type="colorScale" priority="5119">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7228,7 +7233,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:K19 K35 K39:K49 K52:K59 K22:K30">
-    <cfRule type="colorScale" priority="5193">
+    <cfRule type="colorScale" priority="5197">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7240,7 +7245,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:K59 K6:K19 K39:K49 K35 K22:K30">
-    <cfRule type="colorScale" priority="5263">
+    <cfRule type="colorScale" priority="5267">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7252,7 +7257,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:J63">
-    <cfRule type="colorScale" priority="92">
+    <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7264,7 +7269,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66">
-    <cfRule type="colorScale" priority="261">
+    <cfRule type="colorScale" priority="265">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7276,7 +7281,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="colorScale" priority="260">
+    <cfRule type="colorScale" priority="264">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7288,7 +7293,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68">
-    <cfRule type="colorScale" priority="259">
+    <cfRule type="colorScale" priority="263">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7300,7 +7305,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="colorScale" priority="258">
+    <cfRule type="colorScale" priority="262">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7312,7 +7317,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="colorScale" priority="257">
+    <cfRule type="colorScale" priority="261">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7324,7 +7329,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="colorScale" priority="256">
+    <cfRule type="colorScale" priority="260">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7336,7 +7341,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="colorScale" priority="5294">
+    <cfRule type="colorScale" priority="5298">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7348,7 +7353,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71:K71">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7360,7 +7365,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71:K71">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -7368,12 +7373,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="37" priority="47" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="36" priority="48" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="35" priority="49" rank="1"/>
+    <cfRule type="top10" dxfId="37" priority="51" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="36" priority="52" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="35" priority="53" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -7381,12 +7386,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="34" priority="43" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="33" priority="44" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="32" priority="45" rank="1"/>
+    <cfRule type="top10" dxfId="34" priority="47" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="33" priority="48" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="32" priority="49" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:K29">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -7394,12 +7399,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="31" priority="39" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="30" priority="40" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="29" priority="41" rank="1"/>
+    <cfRule type="top10" dxfId="31" priority="43" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="30" priority="44" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="29" priority="45" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:K29">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7411,7 +7416,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:K28">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7423,7 +7428,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:K28">
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -7431,12 +7436,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="28" priority="33" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="27" priority="34" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="26" priority="35" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="37" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="27" priority="38" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="26" priority="39" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -7444,12 +7449,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="25" priority="29" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="24" priority="30" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="23" priority="31" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="33" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="24" priority="34" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="23" priority="35" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7461,7 +7466,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -7469,12 +7474,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="22" priority="24" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="21" priority="25" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="20" priority="26" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="28" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="21" priority="29" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="20" priority="30" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7486,7 +7491,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -7494,12 +7499,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="19" priority="19" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="18" priority="20" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="17" priority="21" rank="1"/>
+    <cfRule type="top10" dxfId="19" priority="23" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="18" priority="24" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="17" priority="25" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7511,7 +7516,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:G29">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -7519,12 +7524,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="16" priority="14" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="15" priority="15" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="14" priority="16" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="18" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="15" priority="19" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="14" priority="20" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:G29">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7536,7 +7541,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="90"/>
@@ -7544,12 +7549,12 @@
         <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="13" priority="9" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="12" priority="10" percent="1" rank="33"/>
-    <cfRule type="top10" dxfId="11" priority="11" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="13" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="12" priority="14" percent="1" rank="33"/>
+    <cfRule type="top10" dxfId="11" priority="15" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7561,7 +7566,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7573,7 +7578,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:K30">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:J22 J23">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22:J23">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Test results (images, XLSX & PDF) are updated.
</commit_message>
<xml_diff>
--- a/_Documents/ORMBattle.NET Test Results.xlsx
+++ b/_Documents/ORMBattle.NET Test Results.xlsx
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="92">
   <si>
     <t>SqlClient</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
   </si>
 </sst>
 </file>
@@ -2624,7 +2627,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2953,25 +2955,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115203456"/>
-        <c:axId val="115500160"/>
+        <c:axId val="114810240"/>
+        <c:axId val="115106944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115203456"/>
+        <c:axId val="114810240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115500160"/>
+        <c:crossAx val="115106944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115500160"/>
+        <c:axId val="115106944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2981,20 +2983,19 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115203456"/>
+        <c:crossAx val="114810240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000588" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000588" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000006" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000006" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3029,7 +3030,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3198,25 +3198,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115533696"/>
-        <c:axId val="115535232"/>
+        <c:axId val="115140480"/>
+        <c:axId val="115142016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115533696"/>
+        <c:axId val="115140480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115535232"/>
+        <c:crossAx val="115142016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115535232"/>
+        <c:axId val="115142016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3225,7 +3225,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115533696"/>
+        <c:crossAx val="115140480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="150000"/>
@@ -3233,13 +3233,12 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000611" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000611" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000622" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000622" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3273,7 +3272,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3490,25 +3488,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115794688"/>
-        <c:axId val="115796224"/>
+        <c:axId val="115397376"/>
+        <c:axId val="115398912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115794688"/>
+        <c:axId val="115397376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115796224"/>
+        <c:crossAx val="115398912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115796224"/>
+        <c:axId val="115398912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,20 +3515,19 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115794688"/>
+        <c:crossAx val="115397376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000588" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000588" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000006" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000006" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3565,7 +3562,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3654,25 +3650,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115419008"/>
-        <c:axId val="115420544"/>
+        <c:axId val="115021696"/>
+        <c:axId val="115023232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115419008"/>
+        <c:axId val="115021696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115420544"/>
+        <c:crossAx val="115023232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115420544"/>
+        <c:axId val="115023232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3681,20 +3677,19 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115419008"/>
+        <c:crossAx val="115021696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000633" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000633" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000644" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000644" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3817,25 +3812,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115448832"/>
-        <c:axId val="115462912"/>
+        <c:axId val="115055616"/>
+        <c:axId val="115069696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115448832"/>
+        <c:axId val="115055616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115462912"/>
+        <c:crossAx val="115069696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115462912"/>
+        <c:axId val="115069696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3846,7 +3841,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115448832"/>
+        <c:crossAx val="115055616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3859,7 +3854,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000611" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000611" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000622" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000622" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3894,7 +3889,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4223,25 +4217,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115900416"/>
-        <c:axId val="115901952"/>
+        <c:axId val="115507200"/>
+        <c:axId val="115508736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115900416"/>
+        <c:axId val="115507200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115901952"/>
+        <c:crossAx val="115508736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115901952"/>
+        <c:axId val="115508736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4250,14 +4244,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115900416"/>
+        <c:crossAx val="115507200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -4273,7 +4266,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000655" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000655" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000666" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000666" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4308,7 +4301,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4637,25 +4629,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="115927680"/>
-        <c:axId val="115945856"/>
+        <c:axId val="115534464"/>
+        <c:axId val="115552640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115927680"/>
+        <c:axId val="115534464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115945856"/>
+        <c:crossAx val="115552640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115945856"/>
+        <c:axId val="115552640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4665,20 +4657,19 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115927680"/>
+        <c:crossAx val="115534464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000611" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000611" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000622" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000622" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5217,8 +5208,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6381,7 +6372,7 @@
       </c>
       <c r="C39" s="40"/>
       <c r="D39" s="69">
-        <v>18738</v>
+        <v>21854</v>
       </c>
       <c r="E39" s="32">
         <v>4634</v>
@@ -6417,7 +6408,9 @@
       </c>
       <c r="B40" s="49"/>
       <c r="C40" s="49"/>
-      <c r="D40" s="63"/>
+      <c r="D40" s="63" t="s">
+        <v>91</v>
+      </c>
       <c r="M40" s="43"/>
     </row>
     <row r="41" spans="1:13" s="32" customFormat="1">
@@ -6429,7 +6422,7 @@
       </c>
       <c r="C41" s="40"/>
       <c r="D41" s="69">
-        <v>10688</v>
+        <v>19043</v>
       </c>
       <c r="E41" s="32">
         <v>4566</v>
@@ -6468,7 +6461,7 @@
       </c>
       <c r="C42" s="40"/>
       <c r="D42" s="69">
-        <v>15379</v>
+        <v>18749</v>
       </c>
       <c r="E42" s="32">
         <v>3898</v>
@@ -6507,7 +6500,7 @@
       </c>
       <c r="C43" s="40"/>
       <c r="D43" s="69">
-        <v>16281</v>
+        <v>19334</v>
       </c>
       <c r="E43" s="32">
         <v>5955</v>
@@ -6546,7 +6539,7 @@
       </c>
       <c r="C44" s="40"/>
       <c r="D44" s="69">
-        <v>13635</v>
+        <v>18655</v>
       </c>
       <c r="E44" s="32">
         <v>4641</v>
@@ -6582,7 +6575,9 @@
       </c>
       <c r="B45" s="49"/>
       <c r="C45" s="49"/>
-      <c r="D45" s="63"/>
+      <c r="D45" s="63" t="s">
+        <v>91</v>
+      </c>
       <c r="M45" s="43"/>
     </row>
     <row r="46" spans="1:13" s="32" customFormat="1">
@@ -6594,7 +6589,7 @@
       </c>
       <c r="C46" s="40"/>
       <c r="D46" s="69">
-        <v>21779</v>
+        <v>61981</v>
       </c>
       <c r="E46" s="32">
         <v>7915</v>
@@ -6633,7 +6628,7 @@
       </c>
       <c r="C47" s="40"/>
       <c r="D47" s="69">
-        <v>64662</v>
+        <v>68567</v>
       </c>
       <c r="E47" s="32">
         <v>6199</v>
@@ -6672,7 +6667,7 @@
       </c>
       <c r="C48" s="40"/>
       <c r="D48" s="69">
-        <v>24219</v>
+        <v>82155</v>
       </c>
       <c r="E48" s="32">
         <v>9365</v>
@@ -6711,7 +6706,7 @@
       </c>
       <c r="C49" s="40"/>
       <c r="D49" s="69">
-        <v>29219</v>
+        <v>69274</v>
       </c>
       <c r="E49" s="32">
         <v>6997</v>
@@ -6861,7 +6856,7 @@
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="69">
-        <v>18745</v>
+        <v>18645</v>
       </c>
       <c r="E55" s="32">
         <v>9728</v>

</xml_diff>